<commit_message>
Changes to the timeout timer based on available parts; updated SCH and BOM. Also fixed off-by-one-row errors for Mouser parts.
</commit_message>
<xml_diff>
--- a/BOM/oresat-c3-BOM.xlsx
+++ b/BOM/oresat-c3-BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26" count="26">
   <si>
     <t>Susumu</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>NO PLACE</t>
   </si>
   <si>
     <t>Murata Electronics</t>
@@ -51,10 +54,10 @@
     <t>Coilcraft</t>
   </si>
   <si>
-    <t>ECS Inc.</t>
+    <t>Delta Electronics/Components</t>
   </si>
   <si>
-    <t>Delta Electronics/Components</t>
+    <t>ECS Inc.</t>
   </si>
   <si>
     <t>ON Semiconductor</t>
@@ -69,31 +72,16 @@
     <t>Vishay Dale</t>
   </si>
   <si>
-    <t>R-US_0402-B-NOSILK</t>
-  </si>
-  <si>
     <t>Bourns</t>
   </si>
   <si>
-    <t>R-US_0603-C-NOSILK</t>
-  </si>
-  <si>
     <t>CRCW040247R0FKED</t>
-  </si>
-  <si>
-    <t>R-US_0402-C-NOSILK</t>
   </si>
   <si>
     <t>Yageo</t>
   </si>
   <si>
     <t>Panasonic Electronic Components</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>47k</t>
   </si>
   <si>
     <t>Micropower 150-mA Low-Noise Ultra-Low-Dropout Regulator in SOT-23 packages</t>
@@ -106,6 +94,9 @@
   </si>
   <si>
     <t>MAC-24+</t>
+  </si>
+  <si>
+    <t>922-500530</t>
   </si>
 </sst>
 </file>
@@ -160,11 +151,7 @@
       <protection locked="1" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
+  <cellXfs count="3">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
@@ -186,296 +173,296 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HV127"/>
+  <dimension ref="A1:HV128"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="75" tabSelected="1">
+    <sheetView workbookViewId="0" zoomScale="85" tabSelected="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
+      <selection pane="bottomLeft" activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" style="1" width="3.9997596153846158" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" style="1" width="33.71225961538462" customWidth="1"/>
-    <col min="3" max="3" style="1" width="24.950881410256414" customWidth="1"/>
-    <col min="4" max="4" style="1" width="30.66482371794872" customWidth="1"/>
-    <col min="5" max="5" style="1" width="72.56706730769231" customWidth="1"/>
-    <col min="6" max="6" style="1" width="27.541201923076926" customWidth="1"/>
-    <col min="7" max="7" style="1" width="32.379006410256416" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" style="1" width="18.856009615384618" customWidth="1"/>
-    <col min="9" max="9" style="1" width="23.808092948717952" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" style="1" width="9.142307692307693"/>
-    <col min="12" max="12" style="1" width="33.90272435897436" customWidth="1"/>
-    <col min="13" max="256" style="1" width="9.142307692307693"/>
+    <col min="1" max="1" style="0" width="3.9997596153846158" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" style="0" width="33.71225961538462" customWidth="1"/>
+    <col min="3" max="3" style="0" width="24.950881410256414" customWidth="1"/>
+    <col min="4" max="4" style="0" width="30.66482371794872" customWidth="1"/>
+    <col min="5" max="5" style="0" width="85.85198317307693" customWidth="1"/>
+    <col min="6" max="6" style="0" width="11.595941742081449" customWidth="1"/>
+    <col min="7" max="7" style="0" width="32.379006410256416" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" style="0" width="14.78902714932127" customWidth="1"/>
+    <col min="9" max="9" style="0" width="23.808092948717952" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" style="0" width="9.142307692307693"/>
+    <col min="12" max="12" style="0" width="33.90272435897436" customWidth="1"/>
+    <col min="13" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:230" ht="13.5">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Parts</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>MFR</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>MPN</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>DIST</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>DPN</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>DIST2</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>DPN2</t>
         </is>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2"/>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="2"/>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
-      <c r="BD1" s="2"/>
-      <c r="BE1" s="2"/>
-      <c r="BF1" s="2"/>
-      <c r="BG1" s="2"/>
-      <c r="BH1" s="2"/>
-      <c r="BI1" s="2"/>
-      <c r="BJ1" s="2"/>
-      <c r="BK1" s="2"/>
-      <c r="BL1" s="2"/>
-      <c r="BM1" s="2"/>
-      <c r="BN1" s="2"/>
-      <c r="BO1" s="2"/>
-      <c r="BP1" s="2"/>
-      <c r="BQ1" s="2"/>
-      <c r="BR1" s="2"/>
-      <c r="BS1" s="2"/>
-      <c r="BT1" s="2"/>
-      <c r="BU1" s="2"/>
-      <c r="BV1" s="2"/>
-      <c r="BW1" s="2"/>
-      <c r="BX1" s="2"/>
-      <c r="BY1" s="2"/>
-      <c r="BZ1" s="2"/>
-      <c r="CA1" s="2"/>
-      <c r="CB1" s="2"/>
-      <c r="CC1" s="2"/>
-      <c r="CD1" s="2"/>
-      <c r="CE1" s="2"/>
-      <c r="CF1" s="2"/>
-      <c r="CG1" s="2"/>
-      <c r="CH1" s="2"/>
-      <c r="CI1" s="2"/>
-      <c r="CJ1" s="2"/>
-      <c r="CK1" s="2"/>
-      <c r="CL1" s="2"/>
-      <c r="CM1" s="2"/>
-      <c r="CN1" s="2"/>
-      <c r="CO1" s="2"/>
-      <c r="CP1" s="2"/>
-      <c r="CQ1" s="2"/>
-      <c r="CR1" s="2"/>
-      <c r="CS1" s="2"/>
-      <c r="CT1" s="2"/>
-      <c r="CU1" s="2"/>
-      <c r="CV1" s="2"/>
-      <c r="CW1" s="2"/>
-      <c r="CX1" s="2"/>
-      <c r="CY1" s="2"/>
-      <c r="CZ1" s="2"/>
-      <c r="DA1" s="2"/>
-      <c r="DB1" s="2"/>
-      <c r="DC1" s="2"/>
-      <c r="DD1" s="2"/>
-      <c r="DE1" s="2"/>
-      <c r="DF1" s="2"/>
-      <c r="DG1" s="2"/>
-      <c r="DH1" s="2"/>
-      <c r="DI1" s="2"/>
-      <c r="DJ1" s="2"/>
-      <c r="DK1" s="2"/>
-      <c r="DL1" s="2"/>
-      <c r="DM1" s="2"/>
-      <c r="DN1" s="2"/>
-      <c r="DO1" s="2"/>
-      <c r="DP1" s="2"/>
-      <c r="DQ1" s="2"/>
-      <c r="DR1" s="2"/>
-      <c r="DS1" s="2"/>
-      <c r="DT1" s="2"/>
-      <c r="DU1" s="2"/>
-      <c r="DV1" s="2"/>
-      <c r="DW1" s="2"/>
-      <c r="DX1" s="2"/>
-      <c r="DY1" s="2"/>
-      <c r="DZ1" s="2"/>
-      <c r="EA1" s="2"/>
-      <c r="EB1" s="2"/>
-      <c r="EC1" s="2"/>
-      <c r="ED1" s="2"/>
-      <c r="EE1" s="2"/>
-      <c r="EF1" s="2"/>
-      <c r="EG1" s="2"/>
-      <c r="EH1" s="2"/>
-      <c r="EI1" s="2"/>
-      <c r="EJ1" s="2"/>
-      <c r="EK1" s="2"/>
-      <c r="EL1" s="2"/>
-      <c r="EM1" s="2"/>
-      <c r="EN1" s="2"/>
-      <c r="EO1" s="2"/>
-      <c r="EP1" s="2"/>
-      <c r="EQ1" s="2"/>
-      <c r="ER1" s="2"/>
-      <c r="ES1" s="2"/>
-      <c r="ET1" s="2"/>
-      <c r="EU1" s="2"/>
-      <c r="EV1" s="2"/>
-      <c r="EW1" s="2"/>
-      <c r="EX1" s="2"/>
-      <c r="EY1" s="2"/>
-      <c r="EZ1" s="2"/>
-      <c r="FA1" s="2"/>
-      <c r="FB1" s="2"/>
-      <c r="FC1" s="2"/>
-      <c r="FD1" s="2"/>
-      <c r="FE1" s="2"/>
-      <c r="FF1" s="2"/>
-      <c r="FG1" s="2"/>
-      <c r="FH1" s="2"/>
-      <c r="FI1" s="2"/>
-      <c r="FJ1" s="2"/>
-      <c r="FK1" s="2"/>
-      <c r="FL1" s="2"/>
-      <c r="FM1" s="2"/>
-      <c r="FN1" s="2"/>
-      <c r="FO1" s="2"/>
-      <c r="FP1" s="2"/>
-      <c r="FQ1" s="2"/>
-      <c r="FR1" s="2"/>
-      <c r="FS1" s="2"/>
-      <c r="FT1" s="2"/>
-      <c r="FU1" s="2"/>
-      <c r="FV1" s="2"/>
-      <c r="FW1" s="2"/>
-      <c r="FX1" s="2"/>
-      <c r="FY1" s="2"/>
-      <c r="FZ1" s="2"/>
-      <c r="GA1" s="2"/>
-      <c r="GB1" s="2"/>
-      <c r="GC1" s="2"/>
-      <c r="GD1" s="2"/>
-      <c r="GE1" s="2"/>
-      <c r="GF1" s="2"/>
-      <c r="GG1" s="2"/>
-      <c r="GH1" s="2"/>
-      <c r="GI1" s="2"/>
-      <c r="GJ1" s="2"/>
-      <c r="GK1" s="2"/>
-      <c r="GL1" s="2"/>
-      <c r="GM1" s="2"/>
-      <c r="GN1" s="2"/>
-      <c r="GO1" s="2"/>
-      <c r="GP1" s="2"/>
-      <c r="GQ1" s="2"/>
-      <c r="GR1" s="2"/>
-      <c r="GS1" s="2"/>
-      <c r="GT1" s="2"/>
-      <c r="GU1" s="2"/>
-      <c r="GV1" s="2"/>
-      <c r="GW1" s="2"/>
-      <c r="GX1" s="2"/>
-      <c r="GY1" s="2"/>
-      <c r="GZ1" s="2"/>
-      <c r="HA1" s="2"/>
-      <c r="HB1" s="2"/>
-      <c r="HC1" s="2"/>
-      <c r="HD1" s="2"/>
-      <c r="HE1" s="2"/>
-      <c r="HF1" s="2"/>
-      <c r="HG1" s="2"/>
-      <c r="HH1" s="2"/>
-      <c r="HI1" s="2"/>
-      <c r="HJ1" s="2"/>
-      <c r="HK1" s="2"/>
-      <c r="HL1" s="2"/>
-      <c r="HM1" s="2"/>
-      <c r="HN1" s="2"/>
-      <c r="HO1" s="2"/>
-      <c r="HP1" s="2"/>
-      <c r="HQ1" s="2"/>
-      <c r="HR1" s="2"/>
-      <c r="HS1" s="2"/>
-      <c r="HT1" s="2"/>
-      <c r="HU1" s="2"/>
-      <c r="HV1" s="2"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="1"/>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="1"/>
+      <c r="BC1" s="1"/>
+      <c r="BD1" s="1"/>
+      <c r="BE1" s="1"/>
+      <c r="BF1" s="1"/>
+      <c r="BG1" s="1"/>
+      <c r="BH1" s="1"/>
+      <c r="BI1" s="1"/>
+      <c r="BJ1" s="1"/>
+      <c r="BK1" s="1"/>
+      <c r="BL1" s="1"/>
+      <c r="BM1" s="1"/>
+      <c r="BN1" s="1"/>
+      <c r="BO1" s="1"/>
+      <c r="BP1" s="1"/>
+      <c r="BQ1" s="1"/>
+      <c r="BR1" s="1"/>
+      <c r="BS1" s="1"/>
+      <c r="BT1" s="1"/>
+      <c r="BU1" s="1"/>
+      <c r="BV1" s="1"/>
+      <c r="BW1" s="1"/>
+      <c r="BX1" s="1"/>
+      <c r="BY1" s="1"/>
+      <c r="BZ1" s="1"/>
+      <c r="CA1" s="1"/>
+      <c r="CB1" s="1"/>
+      <c r="CC1" s="1"/>
+      <c r="CD1" s="1"/>
+      <c r="CE1" s="1"/>
+      <c r="CF1" s="1"/>
+      <c r="CG1" s="1"/>
+      <c r="CH1" s="1"/>
+      <c r="CI1" s="1"/>
+      <c r="CJ1" s="1"/>
+      <c r="CK1" s="1"/>
+      <c r="CL1" s="1"/>
+      <c r="CM1" s="1"/>
+      <c r="CN1" s="1"/>
+      <c r="CO1" s="1"/>
+      <c r="CP1" s="1"/>
+      <c r="CQ1" s="1"/>
+      <c r="CR1" s="1"/>
+      <c r="CS1" s="1"/>
+      <c r="CT1" s="1"/>
+      <c r="CU1" s="1"/>
+      <c r="CV1" s="1"/>
+      <c r="CW1" s="1"/>
+      <c r="CX1" s="1"/>
+      <c r="CY1" s="1"/>
+      <c r="CZ1" s="1"/>
+      <c r="DA1" s="1"/>
+      <c r="DB1" s="1"/>
+      <c r="DC1" s="1"/>
+      <c r="DD1" s="1"/>
+      <c r="DE1" s="1"/>
+      <c r="DF1" s="1"/>
+      <c r="DG1" s="1"/>
+      <c r="DH1" s="1"/>
+      <c r="DI1" s="1"/>
+      <c r="DJ1" s="1"/>
+      <c r="DK1" s="1"/>
+      <c r="DL1" s="1"/>
+      <c r="DM1" s="1"/>
+      <c r="DN1" s="1"/>
+      <c r="DO1" s="1"/>
+      <c r="DP1" s="1"/>
+      <c r="DQ1" s="1"/>
+      <c r="DR1" s="1"/>
+      <c r="DS1" s="1"/>
+      <c r="DT1" s="1"/>
+      <c r="DU1" s="1"/>
+      <c r="DV1" s="1"/>
+      <c r="DW1" s="1"/>
+      <c r="DX1" s="1"/>
+      <c r="DY1" s="1"/>
+      <c r="DZ1" s="1"/>
+      <c r="EA1" s="1"/>
+      <c r="EB1" s="1"/>
+      <c r="EC1" s="1"/>
+      <c r="ED1" s="1"/>
+      <c r="EE1" s="1"/>
+      <c r="EF1" s="1"/>
+      <c r="EG1" s="1"/>
+      <c r="EH1" s="1"/>
+      <c r="EI1" s="1"/>
+      <c r="EJ1" s="1"/>
+      <c r="EK1" s="1"/>
+      <c r="EL1" s="1"/>
+      <c r="EM1" s="1"/>
+      <c r="EN1" s="1"/>
+      <c r="EO1" s="1"/>
+      <c r="EP1" s="1"/>
+      <c r="EQ1" s="1"/>
+      <c r="ER1" s="1"/>
+      <c r="ES1" s="1"/>
+      <c r="ET1" s="1"/>
+      <c r="EU1" s="1"/>
+      <c r="EV1" s="1"/>
+      <c r="EW1" s="1"/>
+      <c r="EX1" s="1"/>
+      <c r="EY1" s="1"/>
+      <c r="EZ1" s="1"/>
+      <c r="FA1" s="1"/>
+      <c r="FB1" s="1"/>
+      <c r="FC1" s="1"/>
+      <c r="FD1" s="1"/>
+      <c r="FE1" s="1"/>
+      <c r="FF1" s="1"/>
+      <c r="FG1" s="1"/>
+      <c r="FH1" s="1"/>
+      <c r="FI1" s="1"/>
+      <c r="FJ1" s="1"/>
+      <c r="FK1" s="1"/>
+      <c r="FL1" s="1"/>
+      <c r="FM1" s="1"/>
+      <c r="FN1" s="1"/>
+      <c r="FO1" s="1"/>
+      <c r="FP1" s="1"/>
+      <c r="FQ1" s="1"/>
+      <c r="FR1" s="1"/>
+      <c r="FS1" s="1"/>
+      <c r="FT1" s="1"/>
+      <c r="FU1" s="1"/>
+      <c r="FV1" s="1"/>
+      <c r="FW1" s="1"/>
+      <c r="FX1" s="1"/>
+      <c r="FY1" s="1"/>
+      <c r="FZ1" s="1"/>
+      <c r="GA1" s="1"/>
+      <c r="GB1" s="1"/>
+      <c r="GC1" s="1"/>
+      <c r="GD1" s="1"/>
+      <c r="GE1" s="1"/>
+      <c r="GF1" s="1"/>
+      <c r="GG1" s="1"/>
+      <c r="GH1" s="1"/>
+      <c r="GI1" s="1"/>
+      <c r="GJ1" s="1"/>
+      <c r="GK1" s="1"/>
+      <c r="GL1" s="1"/>
+      <c r="GM1" s="1"/>
+      <c r="GN1" s="1"/>
+      <c r="GO1" s="1"/>
+      <c r="GP1" s="1"/>
+      <c r="GQ1" s="1"/>
+      <c r="GR1" s="1"/>
+      <c r="GS1" s="1"/>
+      <c r="GT1" s="1"/>
+      <c r="GU1" s="1"/>
+      <c r="GV1" s="1"/>
+      <c r="GW1" s="1"/>
+      <c r="GX1" s="1"/>
+      <c r="GY1" s="1"/>
+      <c r="GZ1" s="1"/>
+      <c r="HA1" s="1"/>
+      <c r="HB1" s="1"/>
+      <c r="HC1" s="1"/>
+      <c r="HD1" s="1"/>
+      <c r="HE1" s="1"/>
+      <c r="HF1" s="1"/>
+      <c r="HG1" s="1"/>
+      <c r="HH1" s="1"/>
+      <c r="HI1" s="1"/>
+      <c r="HJ1" s="1"/>
+      <c r="HK1" s="1"/>
+      <c r="HL1" s="1"/>
+      <c r="HM1" s="1"/>
+      <c r="HN1" s="1"/>
+      <c r="HO1" s="1"/>
+      <c r="HP1" s="1"/>
+      <c r="HQ1" s="1"/>
+      <c r="HR1" s="1"/>
+      <c r="HS1" s="1"/>
+      <c r="HT1" s="1"/>
+      <c r="HU1" s="1"/>
+      <c r="HV1" s="1"/>
     </row>
     <row r="2" spans="1:230" ht="13.5">
       <c r="A2">
@@ -499,7 +486,7 @@
           <t>RF Attenuators 10dB  0Hz ~ 10GHz 50 Ohms 100mW 0805 (2012 Metric)</t>
         </is>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
@@ -530,7 +517,7 @@
           <t>RF Attenuators 10dB  0Hz ~ 10GHz 50 Ohms 64mW 0603 (1608 Metric)</t>
         </is>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
@@ -541,11 +528,11 @@
     </row>
     <row r="4" spans="1:230" ht="14">
       <c r="A4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>C140, C141,C144</t>
+          <t>C40, C74, C77, C83, C140, C141,C144</t>
         </is>
       </c>
       <c r="C4" t="s">
@@ -554,10 +541,8 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>NO PLACE</t>
-        </is>
+      <c r="E4" t="s">
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
@@ -576,7 +561,7 @@
         </is>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -607,7 +592,7 @@
         </is>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -638,7 +623,7 @@
         </is>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -669,7 +654,7 @@
         </is>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -700,7 +685,7 @@
         </is>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -731,7 +716,7 @@
         </is>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -762,7 +747,7 @@
         </is>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -793,7 +778,7 @@
         </is>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -824,7 +809,7 @@
         </is>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -855,7 +840,7 @@
         </is>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -886,7 +871,7 @@
         </is>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -917,7 +902,7 @@
         </is>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -948,7 +933,7 @@
         </is>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -979,7 +964,7 @@
         </is>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1010,7 +995,7 @@
         </is>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1041,7 +1026,7 @@
         </is>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1072,7 +1057,7 @@
         </is>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1103,7 +1088,7 @@
         </is>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1134,7 +1119,7 @@
         </is>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1165,7 +1150,7 @@
         </is>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1196,7 +1181,7 @@
         </is>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1260,7 +1245,7 @@
         </is>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1291,7 +1276,7 @@
         </is>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1322,7 +1307,7 @@
         </is>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1353,7 +1338,7 @@
         </is>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1417,7 +1402,7 @@
         </is>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1547,7 +1532,7 @@
         </is>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1568,7 +1553,7 @@
         </is>
       </c>
       <c r="H36" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -1685,20 +1670,20 @@
         </is>
       </c>
       <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0402CS-2N0XGL</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2nH Fixed Inductors 0402 (1005) Unshld 2% 1.04A 70mOhms AECQ2</t>
+        </is>
+      </c>
+      <c r="H40" t="s">
         <v>9</v>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>0402CS-2N0XGL</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Fixed Inductors 0402 (1005) 2nH Unshld 2% 1.04A 70mOhms AECQ2</t>
-        </is>
-      </c>
-      <c r="H40" t="s">
-        <v>8</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -1716,20 +1701,20 @@
         </is>
       </c>
       <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0402CS-3N9XGL</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>3.9nH Fixed Inductors 0402 (1005) Unshld 2% 840mA 66mOhms AECQ2</t>
+        </is>
+      </c>
+      <c r="H41" t="s">
         <v>9</v>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>0402CS-3N9XGL</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Fixed Inductors 0402 (1005) 3.9nH Unshld 2% 840mA 66mOhms AECQ2</t>
-        </is>
-      </c>
-      <c r="H41" t="s">
-        <v>8</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -1747,7 +1732,7 @@
         </is>
       </c>
       <c r="C42" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1768,7 +1753,7 @@
         </is>
       </c>
       <c r="H42" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -1786,20 +1771,20 @@
         </is>
       </c>
       <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0402HP-5N6XGLW</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>5.6nH Fixed Inductors 0402 (1005) Unshld 2% 1.6A 48mOhms</t>
+        </is>
+      </c>
+      <c r="H43" t="s">
         <v>9</v>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>0402HP-5N6XGLW</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Fixed Inductors 0402 (1005) 5.6nH Unshld 2% 1.6A 48mOhms</t>
-        </is>
-      </c>
-      <c r="H43" t="s">
-        <v>8</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -1813,20 +1798,20 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>L2, L17</t>
+          <t>L16, L22</t>
         </is>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>ECS-MPI4040R4-6R8-R</t>
+          <t>LQW18AN10NG10D</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>6.8µH Shielded  Inductor 2.4A 91mOhm Nonstandard </t>
+          <t>10nH Unshielded Wirewound Inductor 650mA 110mOhm Max 0603 (1608 Metric)</t>
         </is>
       </c>
       <c r="F44" t="s">
@@ -1834,30 +1819,30 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>XC2337CT-ND</t>
+          <t>490-6857-1-ND</t>
         </is>
       </c>
     </row>
     <row r="45" spans="1:230" ht="14">
       <c r="A45">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>L16, L22</t>
+          <t>L1, L3, L38, L39</t>
         </is>
       </c>
       <c r="C45" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>LQW18AN10NG10D</t>
+          <t>0402HP-15NXGLW</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>10nH Unshielded Wirewound Inductor 650mA 110mOhm Max 0603 (1608 Metric)</t>
+          <t>15nH Unshielded Wirewound Inductor 1.1A 110mOhm 0402 (1005 Metric)</t>
         </is>
       </c>
       <c r="F45" t="s">
@@ -1865,17 +1850,17 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>490-6857-1-ND</t>
+          <t>2035-1081-1-ND</t>
         </is>
       </c>
     </row>
     <row r="46" spans="1:230" ht="14">
       <c r="A46">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>L1, L3, L38, L39</t>
+          <t>L5, L14</t>
         </is>
       </c>
       <c r="C46" t="s">
@@ -1883,12 +1868,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0402HP-15NXGLW</t>
+          <t>0402HP-18NXGL</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>15nH Unshielded Wirewound Inductor 1.1A 110mOhm 0402 (1005 Metric)</t>
+          <t>18nH Unshielded Wirewound Inductor 900mA 120mOhm 0402 (1005 Metric)</t>
         </is>
       </c>
       <c r="F46" t="s">
@@ -1896,7 +1881,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2035-1081-1-ND</t>
+          <t>2035-1083-1-ND</t>
         </is>
       </c>
     </row>
@@ -1906,20 +1891,20 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>L5, L14</t>
+          <t>L18, L19</t>
         </is>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0402HP-18NXGL</t>
+          <t>LQW18AN22NG0ZD</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>18nH Unshielded Wirewound Inductor 900mA 120mOhm 0402 (1005 Metric)</t>
+          <t>22nH Unshielded Wirewound Inductor 500mA 300mOhm 0603 (1608 Metric) </t>
         </is>
       </c>
       <c r="F47" t="s">
@@ -1927,30 +1912,30 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2035-1083-1-ND</t>
+          <t>490-16284-1-ND</t>
         </is>
       </c>
     </row>
     <row r="48" spans="1:230" ht="14">
       <c r="A48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>L18, L19</t>
+          <t>L32</t>
         </is>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>LQW18AN22NG0ZD</t>
+          <t>LQW2BAN22NG00L</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>22nH Unshielded Wirewound Inductor 500mA 300mOhm 0603 (1608 Metric) </t>
+          <t>22nH Unshielded Wirewound Inductor 1.9A 70mOhm Max 0805 (2015 Metric) </t>
         </is>
       </c>
       <c r="F48" t="s">
@@ -1958,30 +1943,30 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>490-16284-1-ND</t>
+          <t>490-16027-1-ND</t>
         </is>
       </c>
     </row>
     <row r="49" spans="1:230" ht="14">
       <c r="A49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>L32</t>
+          <t>L6, L7, L10, L11</t>
         </is>
       </c>
       <c r="C49" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>LQW2BAN22NG00L</t>
+          <t>LQW15AN43NG8ZD</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>22nH Unshielded Wirewound Inductor 1.9A 70mOhm Max 0805 (2015 Metric) </t>
+          <t>43nH Unshielded Wirewound Inductor 515mA 516mOhm Max 0402 (1005 Metric) </t>
         </is>
       </c>
       <c r="F49" t="s">
@@ -1989,30 +1974,30 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>490-16027-1-ND</t>
+          <t>490-15447-1-ND</t>
         </is>
       </c>
     </row>
     <row r="50" spans="1:230" ht="14">
       <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>L20</t>
+        </is>
+      </c>
+      <c r="C50" t="s">
         <v>4</v>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>L6, L7, L10, L11</t>
-        </is>
-      </c>
-      <c r="C50" t="s">
-        <v>3</v>
-      </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>LQW15AN43NG8ZD</t>
+          <t>LQW18AS47NG0ZD</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>43nH Unshielded Wirewound Inductor 515mA 516mOhm Max 0402 (1005 Metric) </t>
+          <t>47nH Unshielded Wirewound Inductor 600mA 280mOhm Max 0603 (1608 Metric) </t>
         </is>
       </c>
       <c r="F50" t="s">
@@ -2020,100 +2005,100 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>490-15447-1-ND</t>
+          <t>490-15832-1-ND</t>
+        </is>
+      </c>
+      <c r="H50" t="s">
+        <v>9</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>994-0402HP-47NXGLU</t>
         </is>
       </c>
     </row>
     <row r="51" spans="1:230" ht="14">
       <c r="A51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>L20</t>
+          <t>L27, L30</t>
         </is>
       </c>
       <c r="C51" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>LQW18AS47NG0ZD</t>
+          <t>0402HPH-68NXGLW</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>47nH Unshielded Wirewound Inductor 600mA 280mOhm Max 0603 (1608 Metric) </t>
-        </is>
-      </c>
-      <c r="F51" t="s">
-        <v>1</v>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>490-15832-1-ND</t>
+          <t>68nH Fixed Inductors 0402 (1005) Unshld 2% 320mA 1 Ohms</t>
         </is>
       </c>
       <c r="H51" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>994-0402HP-47NXGLU</t>
+          <t>994-0402HPH-68NXGLW</t>
         </is>
       </c>
     </row>
     <row r="52" spans="1:230" ht="14">
       <c r="A52">
+        <v>6</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>L8, L9, L12, L13, L23, L24</t>
+        </is>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>LQW18AN91NG8ZD</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>91nH Unshielded Wirewound Inductor 520mA 540mOhm Max 0603 (1608 Metric) </t>
+        </is>
+      </c>
+      <c r="F52" t="s">
+        <v>1</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>490-15756-1-ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="53" spans="1:230" ht="13.5">
+      <c r="A53">
         <v>2</v>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>L27, L30</t>
-        </is>
-      </c>
-      <c r="C52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>0402HPH-68NXGLW</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>Fixed Inductors 0402 (1005) 68nH Unshld 2% 320mA 1 Ohms</t>
-        </is>
-      </c>
-      <c r="H52" t="s">
-        <v>8</v>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>994-0402HPH-68NXGLW</t>
-        </is>
-      </c>
-    </row>
-    <row r="53" spans="1:230" ht="14">
-      <c r="A53">
-        <v>6</v>
-      </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>L8, L9, L12, L13, L23, L24</t>
+          <t>L2, L17</t>
         </is>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>LQW18AN91NG8ZD</t>
+          <t>ECS-MPI4040R4-6R8-R</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>91nH Unshielded Wirewound Inductor 520mA 540mOhm Max 0603 (1608 Metric) </t>
+          <t>6.8µH Shielded  Inductor 2.4A 91mOhm Nonstandard </t>
         </is>
       </c>
       <c r="F53" t="s">
@@ -2121,7 +2106,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>490-15756-1-ND</t>
+          <t>XC2337CT-ND</t>
         </is>
       </c>
     </row>
@@ -2168,7 +2153,7 @@
         </is>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -2186,6 +2171,14 @@
       <c r="G55" t="inlineStr">
         <is>
           <t>FDMQ86530LCT-ND</t>
+        </is>
+      </c>
+      <c r="H55" t="s">
+        <v>9</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>512-FDMQ86530L</t>
         </is>
       </c>
     </row>
@@ -2221,14 +2214,6 @@
           <t>NTR4101PT1GOSCT-ND</t>
         </is>
       </c>
-      <c r="H56" t="s">
-        <v>8</v>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>512-FDMQ86530L</t>
-        </is>
-      </c>
     </row>
     <row r="57" spans="1:230" ht="13.5">
       <c r="A57">
@@ -2306,7 +2291,7 @@
         </is>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -2327,44 +2312,38 @@
         </is>
       </c>
     </row>
-    <row r="60" spans="1:230" ht="13.5">
+    <row r="60" spans="1:230" ht="14">
       <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>R10, R67, R82</t>
+        </is>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60" t="s">
+        <v>2</v>
+      </c>
+      <c r="G60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:230" ht="13.5">
+      <c r="A61">
         <v>9</v>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B61" t="inlineStr">
         <is>
           <t>R34, R51, R56, R60, R61, R62, R66, R69, R70</t>
-        </is>
-      </c>
-      <c r="C60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>RMCF0402ZT0R00</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>0 Ohms Jumper 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200 Thick Film</t>
-        </is>
-      </c>
-      <c r="F60" t="s">
-        <v>1</v>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>RMCF0402ZT0R00CT-ND</t>
-        </is>
-      </c>
-    </row>
-    <row r="61" spans="1:230" ht="14">
-      <c r="A61">
-        <v>3</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>R74, R96, R97</t>
         </is>
       </c>
       <c r="C61" t="s">
@@ -2372,12 +2351,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>CRCW06030000Z0EAC</t>
+          <t>RMCF0402ZT0R00</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0 Ohms Jumper 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)  Thick Film</t>
+          <t>0 Ohms Jumper 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F61" t="s">
@@ -2385,41 +2364,30 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>541-4012-1-ND</t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>MCS04020Z0000ZE000</t>
-        </is>
-      </c>
-      <c r="K61" s="3">
-        <v>0</v>
-      </c>
-      <c r="L61" t="s">
-        <v>16</v>
+          <t>RMCF0402ZT0R00CT-ND</t>
+        </is>
       </c>
     </row>
     <row r="62" spans="1:230" ht="14">
       <c r="A62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>R18, R23</t>
+          <t>R74, R96, R97</t>
         </is>
       </c>
       <c r="C62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>CR0603-FX-10R0ELF</t>
+          <t>CRCW06030000Z0EAC</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>10 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+          <t>0 Ohms Jumper 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)  Thick Film</t>
         </is>
       </c>
       <c r="F62" t="s">
@@ -2427,43 +2395,31 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>CR0603-FX-10R0ELFCT-ND</t>
-        </is>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>CRCW06030000ZSTB</t>
-        </is>
-      </c>
-      <c r="K62" s="3">
-        <v>0</v>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>R0603-0-OHMS</t>
-        </is>
-      </c>
+          <t>541-4012-1-ND</t>
+        </is>
+      </c>
+      <c r="K62" s="2"/>
     </row>
     <row r="63" spans="1:230" ht="14">
       <c r="A63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>R49</t>
+          <t>R18, R23</t>
         </is>
       </c>
       <c r="C63" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>RMCF0603FT15R0</t>
+          <t>CR0603-FX-10R0ELF</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>15 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>10 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
         </is>
       </c>
       <c r="F63" t="s">
@@ -2471,43 +2427,31 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>RMCF0603FT15R0CT-ND</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>CRCW060310R0FKEB</t>
-        </is>
-      </c>
-      <c r="K63" s="3">
-        <v>10</v>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>R0603-10-OHMS</t>
-        </is>
-      </c>
+          <t>CR0603-FX-10R0ELFCT-ND</t>
+        </is>
+      </c>
+      <c r="K63" s="2"/>
     </row>
     <row r="64" spans="1:230" ht="14">
       <c r="A64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>R47, R59</t>
+          <t>R49</t>
         </is>
       </c>
       <c r="C64" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>RMCF0603FT27R0</t>
+          <t>RMCF0603FT15R0</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>27 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>15 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F64" t="s">
@@ -2515,41 +2459,31 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>RMCF0603FT27R0CT-ND</t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>CRCW060315R0FKEA</t>
-        </is>
-      </c>
-      <c r="K64" s="3">
-        <v>15</v>
-      </c>
-      <c r="L64" t="s">
-        <v>18</v>
-      </c>
+          <t>RMCF0603FT15R0CT-ND</t>
+        </is>
+      </c>
+      <c r="K64" s="2"/>
     </row>
     <row r="65" spans="1:230" ht="14">
       <c r="A65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>R57</t>
+          <t>R47, R59</t>
         </is>
       </c>
       <c r="C65" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>RMCF0603FT39R0</t>
+          <t>RMCF0603FT27R0</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>39 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>27 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F65" t="s">
@@ -2557,39 +2491,31 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>RMCF0603FT39R0CT-ND</t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>CRCW060327R0FKEA</t>
-        </is>
-      </c>
-      <c r="K65" s="3">
-        <v>27</v>
-      </c>
-      <c r="L65" t="s">
-        <v>18</v>
-      </c>
+          <t>RMCF0603FT27R0CT-ND</t>
+        </is>
+      </c>
+      <c r="K65" s="2"/>
     </row>
     <row r="66" spans="1:230" ht="14">
       <c r="A66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>R94, R95</t>
+          <t>R57</t>
         </is>
       </c>
       <c r="C66" t="s">
         <v>15</v>
       </c>
-      <c r="D66" t="s">
-        <v>19</v>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>RMCF0603FT39R0</t>
+        </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>47 Ohms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>39 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F66" t="s">
@@ -2597,43 +2523,29 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>541-47.0LCT-ND</t>
-        </is>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>CRCW060339R0FKEB</t>
-        </is>
-      </c>
-      <c r="K66" s="3">
-        <v>39</v>
-      </c>
-      <c r="L66" t="s">
-        <v>18</v>
-      </c>
+          <t>RMCF0603FT39R0CT-ND</t>
+        </is>
+      </c>
+      <c r="K66" s="2"/>
     </row>
     <row r="67" spans="1:230" ht="14">
       <c r="A67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>R25</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Vishay Thin Film</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>FC0402E50R0BST1</t>
-        </is>
+          <t>R94, R95</t>
+        </is>
+      </c>
+      <c r="C67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" t="s">
+        <v>18</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>50 Ohms ±0.1% 0.05W, 1/20W Chip Resistor 0402 (1005 Metric) RF, High Frequency Thin Film</t>
+          <t>47 Ohms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F67" t="s">
@@ -2641,39 +2553,33 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>FC0402-50BWCT-ND</t>
-        </is>
-      </c>
-      <c r="I67" t="s">
-        <v>19</v>
-      </c>
-      <c r="K67" s="3">
-        <v>47</v>
-      </c>
-      <c r="L67" t="s">
-        <v>20</v>
-      </c>
+          <t>541-47.0LCT-ND</t>
+        </is>
+      </c>
+      <c r="K67" s="2"/>
     </row>
     <row r="68" spans="1:230" ht="14">
       <c r="A68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>R31, R38</t>
-        </is>
-      </c>
-      <c r="C68" t="s">
-        <v>21</v>
+          <t>R25</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Vishay Thin Film</t>
+        </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>RT0402BRD07150RL</t>
+          <t>FC0402E50R0BST1</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>150 Ohms ±0.1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric)  Thin Film</t>
+          <t>50 Ohms ±0.1% 0.05W, 1/20W Chip Resistor 0402 (1005 Metric) RF, High Frequency Thin Film</t>
         </is>
       </c>
       <c r="F68" t="s">
@@ -2681,15 +2587,10 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>YAG4175CT-ND</t>
-        </is>
-      </c>
-      <c r="K68" s="3">
-        <v>50</v>
-      </c>
-      <c r="L68" t="s">
-        <v>20</v>
-      </c>
+          <t>FC0402-50BWCT-ND</t>
+        </is>
+      </c>
+      <c r="K68" s="2"/>
     </row>
     <row r="69" spans="1:230" ht="14">
       <c r="A69">
@@ -2697,20 +2598,20 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>R85, R101</t>
+          <t>R31, R38</t>
         </is>
       </c>
       <c r="C69" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>CR0603-FX-1500ELF</t>
+          <t>RT0402BRD07150RL</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>150 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+          <t>150 Ohms ±0.1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric)  Thin Film</t>
         </is>
       </c>
       <c r="F69" t="s">
@@ -2718,36 +2619,31 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>118-CR0603-FX-1500ELFCT-ND</t>
-        </is>
-      </c>
-      <c r="K69" s="3">
-        <v>150</v>
-      </c>
-      <c r="L69" t="s">
-        <v>20</v>
-      </c>
+          <t>YAG4175CT-ND</t>
+        </is>
+      </c>
+      <c r="K69" s="2"/>
     </row>
     <row r="70" spans="1:230" ht="14">
       <c r="A70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>R50</t>
+          <t>R85, R101</t>
         </is>
       </c>
       <c r="C70" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>RMCF0603FT220R</t>
+          <t>CR0603-FX-1500ELF</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>220 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>150 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
         </is>
       </c>
       <c r="F70" t="s">
@@ -2755,43 +2651,31 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>RMCF0603FT220RCT-ND</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>CRCW0603150RFKEA</t>
-        </is>
-      </c>
-      <c r="K70" s="3">
-        <v>150</v>
-      </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>R0603-150-OHMS</t>
-        </is>
-      </c>
+          <t>118-CR0603-FX-1500ELFCT-ND</t>
+        </is>
+      </c>
+      <c r="K70" s="2"/>
     </row>
     <row r="71" spans="1:230" ht="14">
       <c r="A71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>R33, R39, R76</t>
+          <t>R50</t>
         </is>
       </c>
       <c r="C71" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>RC0603FR-071KL</t>
+          <t>RMCF0603FT220R</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+          <t>220 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F71" t="s">
@@ -2799,41 +2683,31 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>311-1.00KHRCT-ND</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>CRCW0603220RFKEA</t>
-        </is>
-      </c>
-      <c r="K71" s="3">
-        <v>220</v>
-      </c>
-      <c r="L71" t="s">
-        <v>18</v>
-      </c>
+          <t>RMCF0603FT220RCT-ND</t>
+        </is>
+      </c>
+      <c r="K71" s="2"/>
     </row>
     <row r="72" spans="1:230" ht="14">
       <c r="A72">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>R1, R2, R4, R21, R75</t>
+          <t>R33, R39, R76</t>
         </is>
       </c>
       <c r="C72" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>CR0603-FX-2701ELF</t>
+          <t>RC0603FR-071KL</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2.7 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+          <t>1 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
         </is>
       </c>
       <c r="F72" t="s">
@@ -2841,47 +2715,31 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>CR0603-FX-2701ELFCT-ND</t>
-        </is>
-      </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>CRCW06031K00FKEB</t>
-        </is>
-      </c>
-      <c r="K72" s="3" t="inlineStr">
-        <is>
-          <t>1k</t>
-        </is>
-      </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>R0603-1K-OHMS</t>
-        </is>
-      </c>
+          <t>311-1.00KHRCT-ND</t>
+        </is>
+      </c>
+      <c r="K72" s="2"/>
     </row>
     <row r="73" spans="1:230" ht="14">
       <c r="A73">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>R6, R64</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Vishay Beyschlag</t>
-        </is>
+          <t>R1, R2, R4, R21, R75</t>
+        </is>
+      </c>
+      <c r="C73" t="s">
+        <v>17</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>MCT06030C3101FP500</t>
+          <t>CR0603-FX-2701ELF</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>3.1 kOhms ±1% 0.125W, 1/8W Chip Resistor 0603 (1608 Metric) Anti-Sulfur Thin Film</t>
+          <t>2.7 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
         </is>
       </c>
       <c r="F73" t="s">
@@ -2889,45 +2747,33 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>MCT06030C3101FP500-ND</t>
-        </is>
-      </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>CRCW06032K70FKEA</t>
-        </is>
-      </c>
-      <c r="K73" s="3" t="inlineStr">
-        <is>
-          <t>2.7k</t>
-        </is>
-      </c>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>R0603-2.7K-OHMS</t>
-        </is>
-      </c>
+          <t>CR0603-FX-2701ELFCT-ND</t>
+        </is>
+      </c>
+      <c r="K73" s="2"/>
     </row>
     <row r="74" spans="1:230" ht="14">
       <c r="A74">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>R52, R55, R86, R93</t>
-        </is>
-      </c>
-      <c r="C74" t="s">
-        <v>14</v>
+          <t>R6, R64</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Vishay Beyschlag</t>
+        </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>RMCF0603FT5K60</t>
+          <t>MCT06030C3101FP500</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>5.6 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>3.1 kOhms ±1% 0.125W, 1/8W Chip Resistor 0603 (1608 Metric) Anti-Sulfur Thin Film</t>
         </is>
       </c>
       <c r="F74" t="s">
@@ -2935,45 +2781,31 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>RMCF0603FT5K60CT-ND</t>
-        </is>
-      </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>CRCW06033K09FKEA</t>
-        </is>
-      </c>
-      <c r="K74" s="3" t="inlineStr">
-        <is>
-          <t>3.1k</t>
-        </is>
-      </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>R0603-3.1K-OHMS</t>
-        </is>
-      </c>
+          <t>MCT06030C3101FP500-ND</t>
+        </is>
+      </c>
+      <c r="K74" s="2"/>
     </row>
     <row r="75" spans="1:230" ht="14">
       <c r="A75">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>R53, R54</t>
+          <t>R52, R55, R93</t>
         </is>
       </c>
       <c r="C75" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>EMCF0603FT6K80</t>
+          <t>RMCF0603FT5K60</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>6.8 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>5.6 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F75" t="s">
@@ -2981,115 +2813,74 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>EMCF0603FT6K80CT-ND</t>
-        </is>
-      </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>CRCW06035K60FKEA</t>
-        </is>
-      </c>
-      <c r="K75" s="3" t="inlineStr">
-        <is>
-          <t>5.6k</t>
-        </is>
-      </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>R0603-5.6K-OHMS</t>
-        </is>
-      </c>
+          <t>RMCF0603FT5K60CT-ND</t>
+        </is>
+      </c>
+      <c r="K75" s="2"/>
     </row>
     <row r="76" spans="1:230" ht="14">
       <c r="A76">
+        <v>2</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>R53, R54</t>
+        </is>
+      </c>
+      <c r="C76" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>EMCF0603FT6K80</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>6.8 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+        </is>
+      </c>
+      <c r="F76" t="s">
+        <v>1</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>EMCF0603FT6K80CT-ND</t>
+        </is>
+      </c>
+      <c r="K76" s="2"/>
+    </row>
+    <row r="77" spans="1:230" ht="14">
+      <c r="A77">
         <v>27</v>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>R3, R7, R8, R9, R11, R12, R16, R17, R19, R20, R22, R24, R27, R40, R44,R45, R68, R77, R78,  R80, R81, R82, R83, R84, R92, R98, R102</t>
-        </is>
-      </c>
-      <c r="C76" t="s">
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>R3, R7, R8, R9, R11, R12, R16, R17, R19, R20, R22, R24, R27, R40, R44, R45, R68, R77, R78,  R80, R81, R83, R84, R86, R92, R98, R102</t>
+        </is>
+      </c>
+      <c r="C77" t="s">
         <v>17</v>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>CR0603-FX-1002ELF</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
+      <c r="E77" t="inlineStr">
         <is>
           <t>10 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
         </is>
       </c>
-      <c r="F76" t="s">
-        <v>1</v>
-      </c>
-      <c r="G76" t="inlineStr">
+      <c r="F77" t="s">
+        <v>1</v>
+      </c>
+      <c r="G77" t="inlineStr">
         <is>
           <t>CR0603-FX-1002ELFCT-ND</t>
         </is>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>CRCW06036K80FKEB</t>
-        </is>
-      </c>
-      <c r="K76" s="3" t="inlineStr">
-        <is>
-          <t>6.8k</t>
-        </is>
-      </c>
-      <c r="L76" t="inlineStr">
-        <is>
-          <t>R0603-6.8K-OHMS</t>
-        </is>
-      </c>
-    </row>
-    <row r="77" spans="1:230" ht="13.5">
-      <c r="A77">
-        <v>2</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>R14, R15</t>
-        </is>
-      </c>
-      <c r="C77" t="s">
-        <v>22</v>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>EXB-A10P103J</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>10k Ohm ±5% 62.5mW Power Per Element Bussed  Resistor Network/Array ±200ppm/°C 2512 (6432 Metric), Concave, Long Side Terminals</t>
-        </is>
-      </c>
-      <c r="F77" t="s">
-        <v>1</v>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>U7103CT-ND</t>
-        </is>
-      </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>CRCW060310K0FKEA</t>
-        </is>
-      </c>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>R0603-10K-OHMS</t>
-        </is>
-      </c>
+      <c r="K77" s="2"/>
     </row>
     <row r="78" spans="1:230" ht="13.5">
       <c r="A78">
@@ -3097,20 +2888,20 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>R71, R79</t>
+          <t>R14, R15</t>
         </is>
       </c>
       <c r="C78" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>CR0603-FX-1502ELF</t>
+          <t>EXB-A10P103J</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>15 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+          <t>10k Ohm ±5% 62.5mW Power Per Element Bussed  Resistor Network/Array ±200ppm/°C 2512 (6432 Metric), Concave, Long Side Terminals</t>
         </is>
       </c>
       <c r="F78" t="s">
@@ -3118,18 +2909,11 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>CR0603-FX-1502ELFCT-ND</t>
-        </is>
-      </c>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>EXB-A10P391JC_ARRAY_EXBA-M</t>
-        </is>
-      </c>
+          <t>U7103CT-ND</t>
+        </is>
+      </c>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
     </row>
     <row r="79" spans="1:230" ht="13.5">
       <c r="A79">
@@ -3137,20 +2921,20 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>R46, R58</t>
+          <t>R71, R79</t>
         </is>
       </c>
       <c r="C79" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>ERJ-3EKF2202V</t>
+          <t>CR0603-FX-1502ELF</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>22 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>15 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
         </is>
       </c>
       <c r="F79" t="s">
@@ -3158,46 +2942,32 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>P22.0KHCT-ND</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>CRCW060315K0FKEB</t>
-        </is>
-      </c>
-      <c r="J79" s="3"/>
-      <c r="K79" s="3" t="inlineStr">
-        <is>
-          <t>15k</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>R0603-15K-OHMS</t>
-        </is>
-      </c>
+          <t>CR0603-FX-1502ELFCT-ND</t>
+        </is>
+      </c>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
     </row>
     <row r="80" spans="1:230" ht="13.5">
       <c r="A80">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>R36, R72, R73</t>
+          <t>R46, R58</t>
         </is>
       </c>
       <c r="C80" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>CR0603-FX-2372ELF</t>
+          <t>ERJ-3EKF2202V</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>23.7 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+          <t>22 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F80" t="s">
@@ -3205,31 +2975,19 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>CR0603-FX-2372ELF-ND</t>
-        </is>
-      </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>CRCW060322K0FKEA</t>
-        </is>
-      </c>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3" t="inlineStr">
-        <is>
-          <t>22k</t>
-        </is>
-      </c>
-      <c r="L80" t="s">
-        <v>18</v>
-      </c>
+          <t>P22.0KHCT-ND</t>
+        </is>
+      </c>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
     </row>
     <row r="81" spans="1:230" ht="13.5">
       <c r="A81">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>R5, R32</t>
+          <t>R36, R72, R73</t>
         </is>
       </c>
       <c r="C81" t="s">
@@ -3237,12 +2995,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>CR0603-FX-3162ELF</t>
+          <t>CR0603-FX-2372ELF</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>31.6 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+          <t>23.7 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
         </is>
       </c>
       <c r="F81" t="s">
@@ -3250,46 +3008,32 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>CR0603-FX-3162ELFCT-ND</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>CRCW060323K7FKEA</t>
-        </is>
-      </c>
-      <c r="J81" s="3"/>
-      <c r="K81" s="3" t="inlineStr">
-        <is>
-          <t>23.7k</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>R0603-23.7K-OHMS</t>
-        </is>
-      </c>
+          <t>CR0603-FX-2372ELF-ND</t>
+        </is>
+      </c>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
     </row>
     <row r="82" spans="1:230" ht="13.5">
       <c r="A82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>R48</t>
+          <t>R5, R32</t>
         </is>
       </c>
       <c r="C82" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>RMCF0603FT45K3</t>
+          <t>CR0603-FX-3162ELF</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>45.3 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>31.6 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
         </is>
       </c>
       <c r="F82" t="s">
@@ -3297,33 +3041,19 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>RMCF0603FT45K3CT-ND</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>CRCW060331K6FKEA</t>
-        </is>
-      </c>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3" t="inlineStr">
-        <is>
-          <t>31.6K</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>R0603-31.6K-OHMS</t>
-        </is>
-      </c>
+          <t>CR0603-FX-3162ELFCT-ND</t>
+        </is>
+      </c>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
     </row>
     <row r="83" spans="1:230" ht="13.5">
       <c r="A83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>R99, R100</t>
+          <t>R48</t>
         </is>
       </c>
       <c r="C83" t="s">
@@ -3331,12 +3061,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>CRCW040247K0FKED</t>
+          <t>RMCF0603FT45K3</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>47 kOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>45.3 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F83" t="s">
@@ -3344,44 +3074,32 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>541-47.0KLCT-ND</t>
-        </is>
-      </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>CRCW060345K3FKEA</t>
-        </is>
-      </c>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3" t="inlineStr">
-        <is>
-          <t>45.3k</t>
-        </is>
-      </c>
-      <c r="L83" t="s">
-        <v>18</v>
-      </c>
+          <t>RMCF0603FT45K3CT-ND</t>
+        </is>
+      </c>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
     </row>
     <row r="84" spans="1:230" ht="13.5">
       <c r="A84">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>R26, R28, R29, R30</t>
+          <t>R99, R100</t>
         </is>
       </c>
       <c r="C84" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>RC0603FR-0747KL</t>
+          <t>CRCW040247K0FKED</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>47 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+          <t>47 kOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F84" t="s">
@@ -3389,37 +3107,32 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>311-47.0KHRCT-ND</t>
-        </is>
-      </c>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L84" t="s">
-        <v>16</v>
-      </c>
+          <t>541-47.0KLCT-ND</t>
+        </is>
+      </c>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
     </row>
     <row r="85" spans="1:230" ht="13.5">
       <c r="A85">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>R13, R35, R37, R41, R42, R43, R63, R65, R87, R88, R89, R90, R91, R103</t>
+          <t>R26, R28, R29, R30</t>
         </is>
       </c>
       <c r="C85" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>RMCF0603FT100K</t>
+          <t>RC0603FR-0747KL</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>100 kOhms ±5% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+          <t>47 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
         </is>
       </c>
       <c r="F85" t="s">
@@ -3427,123 +3140,105 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>RMCF0603FT100KCT-ND</t>
-        </is>
-      </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>CRCW060347K0FKEB</t>
-        </is>
-      </c>
-      <c r="J85" s="3"/>
-      <c r="K85" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>R-US_0603-B-NOSILK</t>
-        </is>
-      </c>
+          <t>311-47.0KHRCT-ND</t>
+        </is>
+      </c>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
     </row>
     <row r="86" spans="1:230" ht="13.5">
       <c r="A86">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
+          <t>R13, R35, R37, R41, R42, R43, R63, R65, R87, R88, R89, R90, R91, R103</t>
+        </is>
+      </c>
+      <c r="C86" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>RMCF0603FT100K</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>100 kOhms ±5% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+        </is>
+      </c>
+      <c r="F86" t="s">
+        <v>1</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>RMCF0603FT100KCT-ND</t>
+        </is>
+      </c>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+    </row>
+    <row r="87" spans="1:230" ht="13.5">
+      <c r="A87">
+        <v>1</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
           <t>RT1</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C87" t="inlineStr">
         <is>
           <t>TDK Corporation</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
+      <c r="D87" t="inlineStr">
         <is>
           <t>NTCG103JF103FT1S</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="E87" t="inlineStr">
         <is>
           <t>THERMISTOR NTC 10KOHM 3380K 0402</t>
         </is>
       </c>
-      <c r="F86" t="s">
-        <v>1</v>
-      </c>
-      <c r="G86" t="inlineStr">
+      <c r="F87" t="s">
+        <v>1</v>
+      </c>
+      <c r="G87" t="inlineStr">
         <is>
           <t>445-174506-1-ND</t>
         </is>
       </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>CRCW0603100KFKEA</t>
-        </is>
-      </c>
-      <c r="K86" s="3" t="inlineStr">
-        <is>
-          <t>100k</t>
-        </is>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>R0603-100K-OHMS</t>
-        </is>
-      </c>
-    </row>
-    <row r="87" spans="1:230" ht="14">
-      <c r="A87">
-        <v>1</v>
-      </c>
-      <c r="B87" t="inlineStr">
+      <c r="K87" s="2"/>
+    </row>
+    <row r="88" spans="1:230" ht="13.23529411764706">
+      <c r="A88">
+        <v>1</v>
+      </c>
+      <c r="B88" t="inlineStr">
         <is>
           <t>U1</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="C88" t="inlineStr">
         <is>
           <t>Maxim Integrated</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
+      <c r="D88" t="inlineStr">
         <is>
           <t>MAX892LEUA+T</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr">
+      <c r="E88" t="inlineStr">
         <is>
           <t>Power Switch ICs - Power Distribution Current-Limited, High-Side P-Channel Switches with Thermal Shutdown</t>
         </is>
       </c>
-    </row>
-    <row r="88" spans="1:230" ht="13.5">
-      <c r="A88">
-        <v>1</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>U10</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Silicon Labs</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>SI4112-D-GM</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>RF Synthesizer w/ integrated VCOs (IF OUT)</t>
-        </is>
-      </c>
       <c r="H88" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I88" t="inlineStr">
         <is>
@@ -3553,36 +3248,30 @@
     </row>
     <row r="89" spans="1:230" ht="13.5">
       <c r="A89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>U11, U13</t>
-        </is>
-      </c>
-      <c r="C89" t="s">
-        <v>12</v>
+          <t>U10</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Silicon Labs</t>
+        </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>AX5043-1-TW30</t>
+          <t>SI4112-D-GM</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>IC RF TxRx Only General ISM &lt; 1GHz  27MHz ~ 1.05GHz 28-VFQFN Exposed Pad</t>
-        </is>
-      </c>
-      <c r="F89" t="s">
-        <v>1</v>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>AX5043-1-TW30OSCT-ND</t>
+          <t>RF Synthesizer w/ integrated VCOs (IF OUT)</t>
         </is>
       </c>
       <c r="H89" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I89" t="inlineStr">
         <is>
@@ -3596,65 +3285,65 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>U12,U14</t>
+          <t>U11, U13</t>
         </is>
       </c>
       <c r="C90" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>LP2985AIM5-1.8/NOPB</t>
-        </is>
-      </c>
-      <c r="E90" t="s">
-        <v>25</v>
+          <t>AX5043-1-TW30</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>IC RF TxRx Only General ISM &lt; 1GHz  27MHz ~ 1.05GHz 28-VFQFN Exposed Pad</t>
+        </is>
       </c>
       <c r="F90" t="s">
         <v>1</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>LP2985AIM5-1.8/NOPBCT-ND</t>
-        </is>
-      </c>
-      <c r="H90" t="s">
-        <v>8</v>
-      </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>926-2985AIM51.8/NOPB</t>
+          <t>AX5043-1-TW30OSCT-ND</t>
         </is>
       </c>
     </row>
     <row r="91" spans="1:230" ht="13.5">
       <c r="A91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>U15</t>
+          <t>U12,U14</t>
         </is>
       </c>
       <c r="C91" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>856930</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>Filter - SAW, 457.5 MHz, 15 MHz</t>
+          <t>LP2985AIM5-1.8/NOPB</t>
+        </is>
+      </c>
+      <c r="E91" t="s">
+        <v>21</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>LP2985AIM5-1.8/NOPBCT-ND</t>
         </is>
       </c>
       <c r="H91" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>772-856930</t>
+          <t>926-2985AIM51.8/NOPB</t>
         </is>
       </c>
     </row>
@@ -3664,82 +3353,80 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>U16</t>
+          <t>U15</t>
         </is>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
-      </c>
-      <c r="D92" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>856930</t>
+        </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>RF Mixer, Diode Ring, 0.3 - 12 GHz</t>
+          <t>Filter - SAW, 457.5 MHz, 15 MHz</t>
         </is>
       </c>
       <c r="H92" t="s">
-        <v>27</v>
-      </c>
-      <c r="I92" t="s">
-        <v>28</v>
+        <v>9</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>772-856930</t>
+        </is>
       </c>
     </row>
     <row r="93" spans="1:230" ht="13.5">
       <c r="A93">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>U17, U19, U21</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>AVX Corp</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>BP0805A1308ASTR</t>
-        </is>
+          <t>U16</t>
+        </is>
+      </c>
+      <c r="C93" t="s">
+        <v>23</v>
+      </c>
+      <c r="D93" t="s">
+        <v>24</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1.308GHz Frequency Band Pass RF Filter (Radio Frequency) 200MHz Bandwidth 1.2dB 0805 (2012 Metric), 4 PC Pad</t>
-        </is>
-      </c>
-      <c r="F93" t="s">
-        <v>1</v>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>478-12187-1-ND</t>
-        </is>
+          <t>RF Mixer, Diode Ring, 0.3 - 12 GHz</t>
+        </is>
+      </c>
+      <c r="H93" t="s">
+        <v>23</v>
+      </c>
+      <c r="I93" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:230" ht="13.5">
       <c r="A94">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>U18</t>
+          <t>U17, U19, U21</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Qualcomm (RF360 - A Qualcomm &amp; TDK Joint Venture)</t>
+          <t>AVX Corp</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>B39162B8666L210</t>
+          <t>BP0805A1308ASTR</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2.15GHz Frequency GPS RF SAW Filter (Sound Acoustic Wave) 1.5dB 46.84MHz Bandwidth 10-SMD, No Lead</t>
+          <t>1.308GHz Frequency Band Pass RF Filter (Radio Frequency) 200MHz Bandwidth 1.2dB 0805 (2012 Metric), 4 PC Pad</t>
         </is>
       </c>
       <c r="F94" t="s">
@@ -3747,7 +3434,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>B39162B8666L210CT-ND</t>
+          <t>478-12187-1-ND</t>
         </is>
       </c>
     </row>
@@ -3757,20 +3444,22 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>U20</t>
-        </is>
-      </c>
-      <c r="C95" t="s">
-        <v>13</v>
+          <t>U18</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Qualcomm (RF360 - A Qualcomm &amp; TDK Joint Venture)</t>
+        </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>BGB741L7ESDE6327XTSA1‎</t>
+          <t>B39162B8666L210</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>High Performance LNAs</t>
+          <t>2.15GHz Frequency GPS RF SAW Filter (Sound Acoustic Wave) 1.5dB 46.84MHz Bandwidth 10-SMD, No Lead</t>
         </is>
       </c>
       <c r="F95" t="s">
@@ -3778,7 +3467,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>BGB741L7ESDE6327XTSA1CT-ND</t>
+          <t>B39162B8666L210CT-ND</t>
         </is>
       </c>
     </row>
@@ -3788,20 +3477,20 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>U22</t>
+          <t>U20</t>
         </is>
       </c>
       <c r="C96" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>TLV7041DCKR</t>
+          <t>BGB741L7ESDE6327XTSA1‎</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Comparator General Purpose Open Drain SC-70-5</t>
+          <t>High Performance LNAs</t>
         </is>
       </c>
       <c r="F96" t="s">
@@ -3809,7 +3498,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>296-51723-1-ND</t>
+          <t>BGB741L7ESDE6327XTSA1CT-ND</t>
         </is>
       </c>
     </row>
@@ -3819,22 +3508,20 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>U24</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Maximum Integrated</t>
-        </is>
+          <t>U22</t>
+        </is>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>MAX941EUA+</t>
+          <t>TLV7041DCKR</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Comparator with Latch, Shutdown CMOS, Push-Pull, TTL 8-uMAX</t>
+          <t>Comparator General Purpose Open Drain SC-70-5</t>
         </is>
       </c>
       <c r="F97" t="s">
@@ -3842,7 +3529,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>MAX941EUA+-ND</t>
+          <t>296-51723-1-ND</t>
         </is>
       </c>
     </row>
@@ -3852,20 +3539,22 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>U25</t>
-        </is>
-      </c>
-      <c r="C98" t="s">
-        <v>7</v>
+          <t>U24</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Maximum Integrated</t>
+        </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>SN74LVC1G32QDBVRQ1</t>
+          <t>MAX941EUA+</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Automotive Catalog Single 2-Input Positive-OR Gate</t>
+          <t>Comparator with Latch, Shutdown CMOS, Push-Pull, TTL 8-uMAX</t>
         </is>
       </c>
       <c r="F98" t="s">
@@ -3873,7 +3562,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>296-24202-1-ND</t>
+          <t>MAX941EUA+-ND</t>
         </is>
       </c>
     </row>
@@ -3883,20 +3572,20 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>U26</t>
+          <t>U25</t>
         </is>
       </c>
       <c r="C99" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>TPS62112RSAT</t>
+          <t>SN74LVC1G32QDBVRQ1</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>TPS6211x 17-V, 1.5-A, Synchronous Step-Down Converter 5V 16-VQFN</t>
+          <t>Automotive Catalog Single 2-Input Positive-OR Gate</t>
         </is>
       </c>
       <c r="F99" t="s">
@@ -3904,7 +3593,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>296-19717-1-ND</t>
+          <t>296-24202-1-ND</t>
         </is>
       </c>
     </row>
@@ -3914,20 +3603,20 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>U27</t>
+          <t>U26</t>
         </is>
       </c>
       <c r="C100" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>TPS259620DDAT</t>
+          <t>TPS62112RSAT</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>TPS259620   - Latch-off eFuse With Accurate Current Monitor 2A 8-SO PowerPad</t>
+          <t>TPS6211x 17-V, 1.5-A, Synchronous Step-Down Converter 5V 16-VQFN</t>
         </is>
       </c>
       <c r="F100" t="s">
@@ -3935,7 +3624,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>296-TPS259620DDATCT-ND</t>
+          <t>296-19717-1-ND</t>
         </is>
       </c>
     </row>
@@ -3945,26 +3634,28 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>U28</t>
+          <t>U27</t>
         </is>
       </c>
       <c r="C101" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>LP2985AIM5-3.3/NOPB</t>
-        </is>
-      </c>
-      <c r="E101" t="s">
-        <v>25</v>
+          <t>TPS259620DDAT</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>TPS259620   - Latch-off eFuse With Accurate Current Monitor 2A 8-SO PowerPad</t>
+        </is>
       </c>
       <c r="F101" t="s">
         <v>1</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>LP2985AIM5-3.3/NOPBCT-ND</t>
+          <t>296-TPS259620DDATCT-ND</t>
         </is>
       </c>
     </row>
@@ -3974,59 +3665,49 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>U29</t>
+          <t>U28</t>
         </is>
       </c>
       <c r="C102" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>SN74LVC1G11IDCKRQ1</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>IC GATE AND 1CH 3-INP SC70-6</t>
-        </is>
+          <t>LP2985AIM5-3.3/NOPB</t>
+        </is>
+      </c>
+      <c r="E102" t="s">
+        <v>21</v>
       </c>
       <c r="F102" t="s">
         <v>1</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>296-36722-1-ND</t>
-        </is>
-      </c>
-      <c r="H102" t="s">
-        <v>8</v>
-      </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>926-2985AIM53.3/NOPB</t>
+          <t>LP2985AIM5-3.3/NOPBCT-ND</t>
         </is>
       </c>
     </row>
     <row r="103" spans="1:230" ht="13.5">
       <c r="A103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>U2, U3</t>
+          <t>U29</t>
         </is>
       </c>
       <c r="C103" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>TCAN330GDCNT</t>
+          <t>SN74LVC1G11IDCKRQ1</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>1/1 Transceiver  CANbus SOT-23-8</t>
+          <t>IC GATE AND 1CH 3-INP SC70-6</t>
         </is>
       </c>
       <c r="F103" t="s">
@@ -4034,30 +3715,46 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>296-44211-1-ND</t>
+          <t>296-36722-1-ND</t>
+        </is>
+      </c>
+      <c r="H103" t="s">
+        <v>9</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>926-2985AIM53.3/NOPB</t>
         </is>
       </c>
     </row>
     <row r="104" spans="1:230" ht="13.5">
       <c r="A104">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>U30</t>
+          <t>U2, U3</t>
         </is>
       </c>
       <c r="C104" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>TQP7M9105</t>
+          <t>TCAN330GDCNT</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>RF Amplifier 50-1500Mhz 1W 5V P1dB 30dBm @ 940Mhz</t>
+          <t>1/1 Transceiver  CANbus SOT-23-8</t>
+        </is>
+      </c>
+      <c r="F104" t="s">
+        <v>1</v>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>296-44211-1-ND</t>
         </is>
       </c>
     </row>
@@ -4067,24 +3764,24 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>U31</t>
+          <t>U30</t>
         </is>
       </c>
       <c r="C105" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>BDCN-20-13+</t>
+          <t>TQP7M9105</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Bi-Directional Coupler / Signal Conditioning BI-DIR COUP / SURF MT / RoHS</t>
+          <t>RF Amplifier 50-1500Mhz 1W 5V P1dB 30dBm @ 940Mhz</t>
         </is>
       </c>
       <c r="H105" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I105" t="inlineStr">
         <is>
@@ -4094,34 +3791,24 @@
     </row>
     <row r="106" spans="1:230" ht="13.5">
       <c r="A106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>U32, U33</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Analog Devices Inc</t>
-        </is>
+          <t>U31</t>
+        </is>
+      </c>
+      <c r="C106" t="s">
+        <v>23</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>LT5534ESC6#TRPBF</t>
+          <t>BDCN-20-13+</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>RF Detector IC Broadcast Television 50MHz ~ 3GHz -63dBm ~ -3dBm ±1dB 6-VSSOP, SC-88, SOT-363</t>
-        </is>
-      </c>
-      <c r="F106" t="s">
-        <v>1</v>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>LT5534ESC6#TRPBFCT-ND</t>
+          <t>Bi-Directional Coupler / Signal Conditioning BI-DIR COUP / SURF MT / RoHS</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -4137,26 +3824,26 @@
     </row>
     <row r="107" spans="1:230" ht="13.5">
       <c r="A107">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>U34</t>
+          <t>U32, U33</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Micro Crystal AG</t>
+          <t>Analog Devices Inc</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>RV-3028-C7 32.768KHZ 1PPM-TA-QA</t>
+          <t>LT5534ESC6#TRPBF</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Real Time Clock (RTC) IC Clock/Calendar 2B, 43B I²C 8-WCDFN</t>
+          <t>RF Detector IC Broadcast Television 50MHz ~ 3GHz -63dBm ~ -3dBm ±1dB 6-VSSOP, SC-88, SOT-363</t>
         </is>
       </c>
       <c r="F107" t="s">
@@ -4164,7 +3851,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>2195-RV-3028-C732.768KHZ1PPM-TA-QACT-ND</t>
+          <t>LT5534ESC6#TRPBFCT-ND</t>
         </is>
       </c>
     </row>
@@ -4174,94 +3861,96 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
+          <t>U34</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Micro Crystal AG</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>RV-3028-C7 32.768KHZ 1PPM-TA-QA</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Real Time Clock (RTC) IC Clock/Calendar 2B, 43B I²C 8-WCDFN</t>
+        </is>
+      </c>
+      <c r="F108" t="s">
+        <v>1</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>2195-RV-3028-C732.768KHZ1PPM-TA-QACT-ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="109" spans="1:230" ht="13.5">
+      <c r="A109">
+        <v>1</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
           <t>U35</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr">
+      <c r="C109" t="inlineStr">
         <is>
           <t>Cypress Semiconductor Corp</t>
         </is>
       </c>
-      <c r="D108" t="inlineStr">
+      <c r="D109" t="inlineStr">
         <is>
           <t>FM24CL64B-DGTR</t>
         </is>
       </c>
-      <c r="E108" t="inlineStr">
+      <c r="E109" t="inlineStr">
         <is>
           <t>FRAM (Ferroelectric RAM) Memory IC 64Kb (8K x 8) I²C 1MHz 550ns 8-TDFN (4x4.5)</t>
         </is>
       </c>
-      <c r="F108" t="s">
-        <v>1</v>
-      </c>
-      <c r="G108" t="inlineStr">
+      <c r="F109" t="s">
+        <v>1</v>
+      </c>
+      <c r="G109" t="inlineStr">
         <is>
           <t>428-4033-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="109" spans="1:230" ht="14">
-      <c r="A109">
-        <v>1</v>
-      </c>
-      <c r="B109" t="inlineStr">
+    <row r="110" spans="1:230" ht="14">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110" t="inlineStr">
         <is>
           <t>U36</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr">
+      <c r="C110" t="inlineStr">
         <is>
           <t>STMicroelectronics</t>
         </is>
       </c>
-      <c r="D109" t="inlineStr">
+      <c r="D110" t="inlineStr">
         <is>
           <t>STM32F439VIT6</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr">
+      <c r="E110" t="inlineStr">
         <is>
           <t>ARM® Cortex®-M4 STM32F4 Microcontroller IC 32-Bit 180MHz 2MB (2M x 8) FLASH 100-LQFP (14x14)</t>
         </is>
       </c>
-      <c r="F109" t="s">
-        <v>1</v>
-      </c>
-      <c r="G109" t="inlineStr">
+      <c r="F110" t="s">
+        <v>1</v>
+      </c>
+      <c r="G110" t="inlineStr">
         <is>
           <t>497-18552-ND</t>
-        </is>
-      </c>
-    </row>
-    <row r="110" spans="1:230" ht="13.5">
-      <c r="A110">
-        <v>1</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>U4</t>
-        </is>
-      </c>
-      <c r="C110" t="s">
-        <v>7</v>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>TPS259621DDAT</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>TPS259621   - Auto-retry eFuse With Accurate Current Monitor  2A 8-SO PowerPad</t>
-        </is>
-      </c>
-      <c r="F110" t="s">
-        <v>1</v>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>296-TPS259621DDATCT-ND</t>
         </is>
       </c>
     </row>
@@ -4271,20 +3960,20 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>U5</t>
+          <t>U4</t>
         </is>
       </c>
       <c r="C111" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>TPS62111RSAT</t>
+          <t>TPS259621DDAT</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>TPS6211x 17-V, 1.5-A, Positive Fixed 3.3V 16-VQFN </t>
+          <t>TPS259621   - Auto-retry eFuse With Accurate Current Monitor  2A 8-SO PowerPad</t>
         </is>
       </c>
       <c r="F111" t="s">
@@ -4292,63 +3981,71 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>296-20670-1-ND</t>
+          <t>296-TPS259621DDATCT-ND</t>
         </is>
       </c>
     </row>
     <row r="112" spans="1:230" ht="13.5">
       <c r="A112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>U6, U23</t>
+          <t>U5</t>
         </is>
       </c>
       <c r="C112" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>LP2985AIM5-2.5/NOPB</t>
-        </is>
-      </c>
-      <c r="E112" t="s">
-        <v>25</v>
+          <t>TPS62111RSAT</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>TPS6211x 17-V, 1.5-A, Positive Fixed 3.3V 16-VQFN </t>
+        </is>
       </c>
       <c r="F112" t="s">
         <v>1</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>LP2985AIM5-2.5/NOPBCT-ND</t>
+          <t>296-20670-1-ND</t>
         </is>
       </c>
     </row>
     <row r="113" spans="1:230" ht="13.5">
       <c r="A113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>U7</t>
+          <t>U6, U23</t>
         </is>
       </c>
       <c r="C113" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>TLV1704AMPWPSEP</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>Analog Comparators 2.2-V to 36-V, radiation hardened microPower quad comparator in space enhanced plastic 14-TSSOP -55 to 125</t>
+          <t>LP2985AIM5-2.5/NOPB</t>
+        </is>
+      </c>
+      <c r="E113" t="s">
+        <v>21</v>
+      </c>
+      <c r="F113" t="s">
+        <v>1</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>LP2985AIM5-2.5/NOPBCT-ND</t>
         </is>
       </c>
       <c r="H113" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I113" t="inlineStr">
         <is>
@@ -4362,24 +4059,24 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>U8</t>
+          <t>U7</t>
         </is>
       </c>
       <c r="C114" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>QPC1022TR7</t>
+          <t>TLV1704AMPWPSEP</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>RF Switch ICs 5-6000MHz SPDT IL .25dB Iso 39dB</t>
+          <t>Analog Comparators 2.2-V to 36-V, radiation hardened microPower quad comparator in space enhanced plastic 14-TSSOP -55 to 125</t>
         </is>
       </c>
       <c r="H114" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I114" t="inlineStr">
         <is>
@@ -4393,34 +4090,24 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>U9</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>Swissbit</t>
-        </is>
+          <t>U8</t>
+        </is>
+      </c>
+      <c r="C115" t="s">
+        <v>22</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>SFEM016GB1EA1TO-I-GE-121-STD</t>
+          <t>QPC1022TR7</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>eMMC 16GB E-MMC MLC EM-20 IND</t>
-        </is>
-      </c>
-      <c r="F115" t="s">
-        <v>1</v>
-      </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>1052-SFEM016GB1EA1TO-I-GE-121-STD-ND</t>
+          <t>RF Switch ICs 5-6000MHz SPDT IL .25dB Iso 39dB</t>
         </is>
       </c>
       <c r="H115" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I115" t="inlineStr">
         <is>
@@ -4434,20 +4121,22 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>X1</t>
-        </is>
-      </c>
-      <c r="C116" t="s">
-        <v>10</v>
+          <t>U9</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Swissbit</t>
+        </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>ECS-160-10-36Q-ES-TR</t>
+          <t>SFEM016GB1EA1TO-I-GE-121-STD</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>16MHz ±30ppm Crystal 10pF 80 Ohms 4-SMD, No Lead</t>
+          <t>eMMC 16GB E-MMC MLC EM-20 IND</t>
         </is>
       </c>
       <c r="F116" t="s">
@@ -4455,16 +4144,14 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>XC2181CT-ND</t>
+          <t>1052-SFEM016GB1EA1TO-I-GE-121-STD-ND</t>
         </is>
       </c>
       <c r="H116" t="s">
-        <v>8</v>
-      </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>922-500530</t>
-        </is>
+        <v>9</v>
+      </c>
+      <c r="I116" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="117" spans="1:230" ht="13.5">
@@ -4473,22 +4160,20 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>X2</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Abracon LLC</t>
-        </is>
+          <t>X1</t>
+        </is>
+      </c>
+      <c r="C117" t="s">
+        <v>12</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>ABS07-120-32.768KHZ-T</t>
+          <t>ECS-160-10-36Q-ES-TR</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>32.768kHz ±20ppm Crystal 6pF 55 kOhms 2-SMD, No Lead</t>
+          <t>16MHz ±30ppm Crystal 10pF 80 Ohms 4-SMD, No Lead</t>
         </is>
       </c>
       <c r="F117" t="s">
@@ -4496,52 +4181,85 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>535-11937-2-ND</t>
+          <t>XC2181CT-ND</t>
         </is>
       </c>
     </row>
     <row r="118" spans="1:230" ht="13.5">
       <c r="A118">
+        <v>1</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Abracon LLC</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>ABS07-120-32.768KHZ-T</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>32.768kHz ±20ppm Crystal 6pF 55 kOhms 2-SMD, No Lead</t>
+        </is>
+      </c>
+      <c r="F118" t="s">
+        <v>1</v>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>535-11937-2-ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="119" spans="1:230" ht="13.5">
+      <c r="A119">
         <v>2</v>
       </c>
-      <c r="B118" t="inlineStr">
+      <c r="B119" t="inlineStr">
         <is>
           <t>X3,X4</t>
         </is>
       </c>
-      <c r="C118" t="inlineStr">
+      <c r="C119" t="inlineStr">
         <is>
           <t>Taitien</t>
         </is>
       </c>
-      <c r="D118" t="inlineStr">
+      <c r="D119" t="inlineStr">
         <is>
           <t>TYKTBLSANF-16.000000</t>
         </is>
       </c>
-      <c r="E118" t="inlineStr">
+      <c r="E119" t="inlineStr">
         <is>
           <t>16MHz TCXO Clipped Sine Wave Oscillator 1.8V  4-SMD, No Lead</t>
         </is>
       </c>
-      <c r="F118" t="s">
-        <v>1</v>
-      </c>
-      <c r="G118" t="inlineStr">
+      <c r="F119" t="s">
+        <v>1</v>
+      </c>
+      <c r="G119" t="inlineStr">
         <is>
           <t>1664-1323-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="119" spans="1:230" ht="13.5"/>
-    <row r="120" spans="1:230" ht="12.75"/>
+    <row r="120" spans="1:230" ht="13.5"/>
     <row r="121" spans="1:230" ht="12.75"/>
     <row r="122" spans="1:230" ht="12.75"/>
-    <row r="123" spans="1:230" ht="14"/>
-    <row r="124" spans="1:230" ht="12.75"/>
+    <row r="123" spans="1:230" ht="12.75"/>
+    <row r="124" spans="1:230" ht="14"/>
     <row r="125" spans="1:230" ht="12.75"/>
     <row r="126" spans="1:230" ht="12.75"/>
     <row r="127" spans="1:230" ht="12.75"/>
+    <row r="128" spans="1:230" ht="12.75"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>

</xml_diff>

<commit_message>
Minor polishing with Glenn, removed L band TX components, fixed BOM.
</commit_message>
<xml_diff>
--- a/BOM/oresat-c3-BOM.xlsx
+++ b/BOM/oresat-c3-BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24" count="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26" count="26">
   <si>
     <t>Susumu</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>GRM188R61E106KA73D</t>
   </si>
   <si>
     <t>Texas Instruments</t>
@@ -79,6 +82,9 @@
   </si>
   <si>
     <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>MAX892LEUA+T</t>
   </si>
   <si>
     <t>Micropower 150-mA Low-Noise Ultra-Low-Dropout Regulator in SOT-23 packages</t>
@@ -194,8 +200,8 @@
   <dimension ref="A1:XFD128"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="85" tabSelected="1">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -17704,10 +17710,8 @@
       <c r="C29" t="s">
         <v>4</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>GRM188R61E106KA73D</t>
-        </is>
+      <c r="D29" t="s">
+        <v>8</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -34304,7 +34308,7 @@
         </is>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -34325,7 +34329,7 @@
         </is>
       </c>
       <c r="H36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -34442,7 +34446,7 @@
         </is>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -34455,7 +34459,7 @@
         </is>
       </c>
       <c r="H40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -34473,7 +34477,7 @@
         </is>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -34486,7 +34490,7 @@
         </is>
       </c>
       <c r="H41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -34525,7 +34529,7 @@
         </is>
       </c>
       <c r="H42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -34543,7 +34547,7 @@
         </is>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -34556,7 +34560,7 @@
         </is>
       </c>
       <c r="H43" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -34605,7 +34609,7 @@
         </is>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -34636,7 +34640,7 @@
         </is>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -34781,7 +34785,7 @@
         </is>
       </c>
       <c r="H50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -34799,7 +34803,7 @@
         </is>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -34812,7 +34816,7 @@
         </is>
       </c>
       <c r="H51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -34861,7 +34865,7 @@
         </is>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -34925,7 +34929,7 @@
         </is>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -34946,7 +34950,7 @@
         </is>
       </c>
       <c r="H55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
@@ -35063,7 +35067,7 @@
         </is>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -35119,7 +35123,7 @@
         </is>
       </c>
       <c r="C61" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -35150,7 +35154,7 @@
         </is>
       </c>
       <c r="C62" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -35182,7 +35186,7 @@
         </is>
       </c>
       <c r="C63" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -35214,7 +35218,7 @@
         </is>
       </c>
       <c r="C64" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D64" s="4" t="inlineStr">
         <is>
@@ -51622,7 +51626,7 @@
         </is>
       </c>
       <c r="C65" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -51654,7 +51658,7 @@
         </is>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -51686,7 +51690,7 @@
         </is>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -51752,7 +51756,7 @@
         </is>
       </c>
       <c r="C69" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -51784,7 +51788,7 @@
         </is>
       </c>
       <c r="C70" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -51816,7 +51820,7 @@
         </is>
       </c>
       <c r="C71" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -51848,7 +51852,7 @@
         </is>
       </c>
       <c r="C72" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -51880,7 +51884,7 @@
         </is>
       </c>
       <c r="C73" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -51911,19 +51915,17 @@
           <t>R6</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Vishay Beyschlag</t>
-        </is>
+      <c r="C74" t="s">
+        <v>16</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>MCT06030C3101FP500</t>
+          <t>RMCF0603FT3K00</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>3.1 kOhms ±1% 0.125W, 1/8W Chip Resistor 0603 (1608 Metric) Anti-Sulfur Thin Film</t>
+          <t>3 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
         </is>
       </c>
       <c r="F74" t="s">
@@ -51931,7 +51933,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>MCT06030C3101FP500-ND</t>
+          <t>RMCF0603FT3K00CT-ND</t>
         </is>
       </c>
       <c r="K74" s="2"/>
@@ -51946,7 +51948,7 @@
         </is>
       </c>
       <c r="C75" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -51978,11 +51980,11 @@
         </is>
       </c>
       <c r="C76" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>EMCF0603FT6K80</t>
+          <t>RMCF0603FT6K80</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -51995,7 +51997,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>EMCF0603FT6K80CT-ND</t>
+          <t>RMCF0603FT6K80CT-ND</t>
         </is>
       </c>
       <c r="K76" s="2"/>
@@ -52010,7 +52012,7 @@
         </is>
       </c>
       <c r="C77" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -52042,7 +52044,7 @@
         </is>
       </c>
       <c r="C78" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -52075,7 +52077,7 @@
         </is>
       </c>
       <c r="C79" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -52108,7 +52110,7 @@
         </is>
       </c>
       <c r="C80" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -52141,11 +52143,11 @@
         </is>
       </c>
       <c r="C81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>CR0603-FX-2372ELF</t>
+          <t>RMCF0603FT23K7</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -52158,7 +52160,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>CR0603-FX-2372ELF-ND</t>
+          <t>RMCF0603FT23K7CT-ND</t>
         </is>
       </c>
       <c r="J81" s="2"/>
@@ -52174,7 +52176,7 @@
         </is>
       </c>
       <c r="C82" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -52207,7 +52209,7 @@
         </is>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -52240,7 +52242,7 @@
         </is>
       </c>
       <c r="C84" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -52273,7 +52275,7 @@
         </is>
       </c>
       <c r="C85" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -52306,7 +52308,7 @@
         </is>
       </c>
       <c r="C86" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D86" s="4" t="inlineStr">
         <is>
@@ -68752,18 +68754,24 @@
           <t>Maxim Integrated</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>MAX892LEUA+T</t>
-        </is>
+      <c r="D88" t="s">
+        <v>21</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
           <t>Power Switch ICs - Power Distribution Current-Limited, High-Side P-Channel Switches with Thermal Shutdown</t>
         </is>
       </c>
+      <c r="F88" t="s">
+        <v>1</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>MAX892LEUA+-ND</t>
+        </is>
+      </c>
       <c r="H88" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I88" t="inlineStr">
         <is>
@@ -68796,7 +68804,7 @@
         </is>
       </c>
       <c r="H89" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I89" t="inlineStr">
         <is>
@@ -68814,7 +68822,7 @@
         </is>
       </c>
       <c r="C90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -68845,7 +68853,7 @@
         </is>
       </c>
       <c r="C91" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -68853,7 +68861,7 @@
         </is>
       </c>
       <c r="E91" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F91" t="s">
         <v>1</v>
@@ -68864,7 +68872,7 @@
         </is>
       </c>
       <c r="H91" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I91" t="inlineStr">
         <is>
@@ -68882,7 +68890,7 @@
         </is>
       </c>
       <c r="C92" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -68895,7 +68903,7 @@
         </is>
       </c>
       <c r="H92" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I92" t="inlineStr">
         <is>
@@ -68913,10 +68921,10 @@
         </is>
       </c>
       <c r="C93" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D93" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -68924,10 +68932,10 @@
         </is>
       </c>
       <c r="H93" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I93" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:16384" ht="13.5">
@@ -69006,7 +69014,7 @@
         </is>
       </c>
       <c r="C96" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -69037,7 +69045,7 @@
         </is>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -69101,7 +69109,7 @@
         </is>
       </c>
       <c r="C99" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -69132,7 +69140,7 @@
         </is>
       </c>
       <c r="C100" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -69163,7 +69171,7 @@
         </is>
       </c>
       <c r="C101" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -69194,7 +69202,7 @@
         </is>
       </c>
       <c r="C102" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -69202,7 +69210,7 @@
         </is>
       </c>
       <c r="E102" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F102" t="s">
         <v>1</v>
@@ -69223,7 +69231,7 @@
         </is>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -69244,7 +69252,7 @@
         </is>
       </c>
       <c r="H103" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I103" t="inlineStr">
         <is>
@@ -69262,7 +69270,7 @@
         </is>
       </c>
       <c r="C104" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -69293,7 +69301,7 @@
         </is>
       </c>
       <c r="C105" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -69306,7 +69314,7 @@
         </is>
       </c>
       <c r="H105" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I105" t="inlineStr">
         <is>
@@ -69324,7 +69332,7 @@
         </is>
       </c>
       <c r="C106" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -69489,7 +69497,7 @@
         </is>
       </c>
       <c r="C111" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -69520,7 +69528,7 @@
         </is>
       </c>
       <c r="C112" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -69551,7 +69559,7 @@
         </is>
       </c>
       <c r="C113" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -69559,7 +69567,7 @@
         </is>
       </c>
       <c r="E113" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F113" t="s">
         <v>1</v>
@@ -69570,7 +69578,7 @@
         </is>
       </c>
       <c r="H113" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I113" t="inlineStr">
         <is>
@@ -69588,7 +69596,7 @@
         </is>
       </c>
       <c r="C114" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -69601,7 +69609,7 @@
         </is>
       </c>
       <c r="H114" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I114" t="inlineStr">
         <is>
@@ -69619,7 +69627,7 @@
         </is>
       </c>
       <c r="C115" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -69632,7 +69640,7 @@
         </is>
       </c>
       <c r="H115" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I115" t="inlineStr">
         <is>
@@ -69673,7 +69681,7 @@
         </is>
       </c>
       <c r="H116" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I116" t="inlineStr">
         <is>
@@ -69691,7 +69699,7 @@
         </is>
       </c>
       <c r="C117" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -69741,7 +69749,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>535-11937-2-ND</t>
+          <t>535-11937-1-ND</t>
         </is>
       </c>
     </row>

</xml_diff>